<commit_message>
Changed all FMOD events to 2D; deleted audio sources from GameObjects; saved and closed projects
</commit_message>
<xml_diff>
--- a/Documentation/AssetList.xlsx
+++ b/Documentation/AssetList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katarinatretter/Documents/GitHub/IGME671/igme671FinalProject/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADCE40F-09FE-F348-9FF4-10C0E44FEAC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B315B69-29D0-7548-A785-E75BDCB127C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10740" windowWidth="16800" windowHeight="10260" xr2:uid="{1AC97BA3-372B-A34D-A085-5D3F8318D120}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{1AC97BA3-372B-A34D-A085-5D3F8318D120}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -744,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FAEC0A-8FA9-B842-819A-74AAE62CF2E8}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>